<commit_message>
added changes - 1st prod version
added changes that were made on prod.
</commit_message>
<xml_diff>
--- a/Exceloutput/error.xlsx
+++ b/Exceloutput/error.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Revert "added changes - 1st prod version"
This reverts commit c4161a7985d9bc108ad85cfc08fbc75348d07a88.
</commit_message>
<xml_diff>
--- a/Exceloutput/error.xlsx
+++ b/Exceloutput/error.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Revert "prototype prod v1"
This reverts commit 61bf22e2af300b22276abf8729c7200cdbaf5afc.
</commit_message>
<xml_diff>
--- a/Exceloutput/error.xlsx
+++ b/Exceloutput/error.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="תעסוקה בישראל" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-ערך התןצר (מיליון דולר)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחהבסקטורביחסלרבעוןמקביל(%)" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב לפי סקטור  (%)" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-במ&quot;ד" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-צמיחה ביחס לאשתקד" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="הרכב רשפ שנתי-הרכב" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הכנסות " sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-הוצאות" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מאזן-מימון גירעון תקציבי" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-מדד" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש המקביל" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="מדד-שינוי במדד ביחס לחודש הקודם" sheetId="13" state="visible" r:id="rId13"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>